<commit_message>
[report] adding analysis, with SHAP both with and without lags
</commit_message>
<xml_diff>
--- a/report/slides/planning_gantt.xlsx
+++ b/report/slides/planning_gantt.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10719"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10811"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/pedrobedmar/GoogleDrive/MASTER_BIG_DATA/tfm/code/report/slides/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB17E9CB-3B65-BA4A-876A-90D89E0CD336}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A7552CB4-DB14-F749-A336-F9D203006CA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="16480" xr2:uid="{10DE0777-76C8-A741-868A-98CED475A390}"/>
+    <workbookView xWindow="38400" yWindow="9020" windowWidth="28800" windowHeight="16480" xr2:uid="{10DE0777-76C8-A741-868A-98CED475A390}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -99,9 +99,6 @@
     <t>Sprint 8</t>
   </si>
   <si>
-    <t>Semana de exámenes</t>
-  </si>
-  <si>
     <t>July</t>
   </si>
   <si>
@@ -109,6 +106,10 @@
   </si>
   <si>
     <t>Sprint 10</t>
+  </si>
+  <si>
+    <t>Exam's 
+week</t>
   </si>
 </sst>
 </file>
@@ -341,7 +342,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="42">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
@@ -372,38 +373,37 @@
     <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="4" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="2" fillId="6" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="6" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
   </cellXfs>
@@ -722,39 +722,39 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1AA6F6FA-264C-CF45-9D61-358A195CF6F3}">
   <dimension ref="B8:L16"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" zoomScale="175" workbookViewId="0">
-      <selection activeCell="F16" sqref="F16"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A2" zoomScale="175" workbookViewId="0">
+      <selection activeCell="B6" sqref="B6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="8" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B8" s="31" t="s">
+      <c r="B8" s="39" t="s">
         <v>18</v>
       </c>
-      <c r="C8" s="28" t="s">
+      <c r="C8" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="D8" s="29"/>
-      <c r="E8" s="29" t="s">
+      <c r="D8" s="37"/>
+      <c r="E8" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="F8" s="29"/>
-      <c r="G8" s="29" t="s">
+      <c r="F8" s="37"/>
+      <c r="G8" s="37" t="s">
         <v>2</v>
       </c>
-      <c r="H8" s="29"/>
-      <c r="I8" s="30" t="s">
+      <c r="H8" s="37"/>
+      <c r="I8" s="38" t="s">
         <v>10</v>
       </c>
-      <c r="J8" s="30"/>
-      <c r="K8" s="40" t="s">
-        <v>21</v>
-      </c>
-      <c r="L8" s="41"/>
+      <c r="J8" s="38"/>
+      <c r="K8" s="31" t="s">
+        <v>20</v>
+      </c>
+      <c r="L8" s="32"/>
     </row>
     <row r="9" spans="2:12" x14ac:dyDescent="0.2">
-      <c r="B9" s="32"/>
+      <c r="B9" s="40"/>
       <c r="C9" s="1" t="s">
         <v>11</v>
       </c>
@@ -780,10 +780,10 @@
         <v>19</v>
       </c>
       <c r="K9" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="L9" s="1" t="s">
         <v>22</v>
-      </c>
-      <c r="L9" s="1" t="s">
-        <v>23</v>
       </c>
     </row>
     <row r="10" spans="2:12" x14ac:dyDescent="0.2">
@@ -794,8 +794,8 @@
       <c r="D10" s="12"/>
       <c r="E10" s="13"/>
       <c r="G10" s="4"/>
-      <c r="H10" s="37" t="s">
-        <v>20</v>
+      <c r="H10" s="33" t="s">
+        <v>23</v>
       </c>
       <c r="I10" s="4"/>
       <c r="J10" s="4"/>
@@ -810,10 +810,10 @@
       <c r="E11" s="14"/>
       <c r="F11" s="15"/>
       <c r="G11" s="7"/>
-      <c r="H11" s="38"/>
+      <c r="H11" s="34"/>
       <c r="I11" s="7"/>
-      <c r="J11" s="33"/>
-      <c r="K11" s="33"/>
+      <c r="J11" s="7"/>
+      <c r="K11" s="7"/>
       <c r="L11" s="8"/>
     </row>
     <row r="12" spans="2:12" x14ac:dyDescent="0.2">
@@ -825,10 +825,10 @@
       <c r="E12" s="18"/>
       <c r="F12" s="19"/>
       <c r="G12" s="7"/>
-      <c r="H12" s="38"/>
+      <c r="H12" s="34"/>
       <c r="I12" s="7"/>
-      <c r="J12" s="33"/>
-      <c r="K12" s="33"/>
+      <c r="J12" s="7"/>
+      <c r="K12" s="7"/>
       <c r="L12" s="8"/>
     </row>
     <row r="13" spans="2:12" x14ac:dyDescent="0.2">
@@ -839,10 +839,10 @@
       <c r="D13" s="7"/>
       <c r="E13" s="16"/>
       <c r="F13" s="17"/>
-      <c r="G13" s="35"/>
-      <c r="H13" s="38"/>
+      <c r="G13" s="29"/>
+      <c r="H13" s="34"/>
       <c r="I13" s="7"/>
-      <c r="J13" s="33"/>
+      <c r="J13" s="7"/>
       <c r="K13" s="10"/>
       <c r="L13" s="8"/>
     </row>
@@ -852,7 +852,7 @@
       </c>
       <c r="C14" s="6"/>
       <c r="D14" s="7"/>
-      <c r="H14" s="38"/>
+      <c r="H14" s="34"/>
       <c r="I14" s="20"/>
       <c r="J14" s="21"/>
       <c r="K14" s="23"/>
@@ -866,10 +866,10 @@
       <c r="D15" s="7"/>
       <c r="E15" s="7"/>
       <c r="F15" s="7"/>
-      <c r="H15" s="38"/>
-      <c r="I15" s="34"/>
+      <c r="H15" s="34"/>
+      <c r="I15" s="28"/>
       <c r="J15" s="8"/>
-      <c r="K15" s="36"/>
+      <c r="K15" s="30"/>
       <c r="L15" s="22"/>
     </row>
     <row r="16" spans="2:12" x14ac:dyDescent="0.2">
@@ -881,7 +881,7 @@
       <c r="E16" s="10"/>
       <c r="F16" s="10"/>
       <c r="G16" s="10"/>
-      <c r="H16" s="39"/>
+      <c r="H16" s="35"/>
       <c r="I16" s="25"/>
       <c r="J16" s="26"/>
       <c r="K16" s="26"/>
@@ -889,13 +889,13 @@
     </row>
   </sheetData>
   <mergeCells count="7">
+    <mergeCell ref="B8:B9"/>
     <mergeCell ref="K8:L8"/>
     <mergeCell ref="H10:H16"/>
     <mergeCell ref="C8:D8"/>
     <mergeCell ref="E8:F8"/>
     <mergeCell ref="I8:J8"/>
     <mergeCell ref="G8:H8"/>
-    <mergeCell ref="B8:B9"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>